<commit_message>
just test main method
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiril\IdeaProjects\TestRequester\Requester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiril\IdeaProjects\TestRequester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DCCF8A-1E73-4A4F-AEC0-8B5CE7982406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A65BE6-035D-43BE-BF7C-69A6B94CCCDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>p</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>transactions</t>
+  </si>
+  <si>
+    <t>jsaf123jlsa513j</t>
+  </si>
+  <si>
+    <t>SLA breached for HITBTC tech issue</t>
+  </si>
+  <si>
+    <t>vbzsdfgdsg1234</t>
+  </si>
+  <si>
+    <t>SLA breached for binance tech issue</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -348,28 +360,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>